<commit_message>
Se termino de pasar todos los datos a la hoja del dr Rolando
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0.xlsx
+++ b/pruebas_excel/marco3Ddam0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05F38DC-B0D0-425C-93FB-0FB71C46B149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD923788-D4FF-4CF8-AF82-876693879AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1815" windowWidth="24240" windowHeight="13740" tabRatio="999" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
+    <workbookView xWindow="28680" yWindow="1815" windowWidth="24240" windowHeight="13740" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="nudos" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="81">
   <si>
     <t>Marco 3D</t>
   </si>
@@ -310,9 +310,6 @@
   </si>
   <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>FSec1</t>
   </si>
   <si>
     <t>circular</t>
@@ -13602,8 +13599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64754D5-97CF-43AF-A87E-0A6E620C6CCD}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13614,83 +13611,101 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
         <v>0</v>
-      </c>
-      <c r="B1">
-        <v>5000</v>
       </c>
       <c r="C1">
         <v>5000</v>
       </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>5000</v>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>5000</v>
+      </c>
+      <c r="D4">
+        <v>5000</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6000</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
         <v>5000</v>
       </c>
-      <c r="C5" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
         <v>6000</v>
       </c>
-      <c r="B6" s="4">
+      <c r="C6" s="4">
         <v>0</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D6" s="4">
         <v>5000</v>
       </c>
-      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
         <v>6000</v>
       </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
       <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>5000</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5000</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
@@ -75098,10 +75113,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D051BC6-55A0-4B3B-BADC-15C4CA1EE579}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:A9"/>
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75111,49 +75126,103 @@
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7071.07</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7810.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9273.6200000000008</v>
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -75166,7 +75235,7 @@
   <dimension ref="A1:Q182"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I9"/>
+      <selection sqref="A1:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75181,8 +75250,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
-        <v>79</v>
+      <c r="A1" s="6">
+        <v>1</v>
       </c>
       <c r="B1" s="8">
         <v>11721.3</v>
@@ -75196,28 +75265,38 @@
       <c r="E1" s="8">
         <v>241862797.40000001</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="8">
+        <v>199947.98</v>
+      </c>
+      <c r="G1" s="8">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" s="6">
+      <c r="J1" s="6">
+        <v>300</v>
+      </c>
+      <c r="K1" s="6">
+        <v>300</v>
+      </c>
+      <c r="L1" s="6">
+        <v>13</v>
+      </c>
+      <c r="M1" s="6">
         <v>7.8090000000000006E-9</v>
       </c>
-      <c r="I1" s="6">
+      <c r="N1" s="6">
         <v>0.65</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
       <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>79</v>
+      <c r="A2" s="6">
+        <v>2</v>
       </c>
       <c r="B2" s="8">
         <v>11721.3</v>
@@ -75231,27 +75310,37 @@
       <c r="E2" s="8">
         <v>241862797.40000001</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="8">
+        <v>199947.98</v>
+      </c>
+      <c r="G2" s="8">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="J2" s="6">
+        <v>300</v>
+      </c>
+      <c r="K2" s="6">
+        <v>300</v>
+      </c>
+      <c r="L2" s="6">
+        <v>13</v>
+      </c>
+      <c r="M2" s="6">
         <v>7.8090000000000006E-9</v>
       </c>
-      <c r="I2" s="6">
+      <c r="N2" s="6">
         <v>0.65</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>79</v>
+      <c r="A3" s="6">
+        <v>3</v>
       </c>
       <c r="B3" s="8">
         <v>11721.3</v>
@@ -75265,27 +75354,37 @@
       <c r="E3" s="8">
         <v>241862797.40000001</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="8">
+        <v>199947.98</v>
+      </c>
+      <c r="G3" s="8">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="J3" s="6">
+        <v>300</v>
+      </c>
+      <c r="K3" s="6">
+        <v>300</v>
+      </c>
+      <c r="L3" s="6">
+        <v>13</v>
+      </c>
+      <c r="M3" s="6">
         <v>7.8090000000000006E-9</v>
       </c>
-      <c r="I3" s="6">
+      <c r="N3" s="6">
         <v>0.65</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>79</v>
+      <c r="A4" s="6">
+        <v>4</v>
       </c>
       <c r="B4" s="8">
         <v>11721.3</v>
@@ -75299,27 +75398,37 @@
       <c r="E4" s="8">
         <v>241862797.40000001</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="8">
+        <v>199947.98</v>
+      </c>
+      <c r="G4" s="8">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="J4" s="6">
+        <v>300</v>
+      </c>
+      <c r="K4" s="6">
+        <v>300</v>
+      </c>
+      <c r="L4" s="6">
+        <v>13</v>
+      </c>
+      <c r="M4" s="6">
         <v>7.8090000000000006E-9</v>
       </c>
-      <c r="I4" s="6">
+      <c r="N4" s="6">
         <v>0.65</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>79</v>
+      <c r="A5" s="6">
+        <v>5</v>
       </c>
       <c r="B5" s="9">
         <v>11721.3</v>
@@ -75333,27 +75442,37 @@
       <c r="E5" s="9">
         <v>241862797.40000001</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G5" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="J5" s="6">
+        <v>300</v>
+      </c>
+      <c r="K5" s="6">
+        <v>300</v>
+      </c>
+      <c r="L5" s="6">
+        <v>13</v>
+      </c>
+      <c r="M5" s="6">
         <v>7.8090000000000006E-9</v>
       </c>
-      <c r="I5" s="6">
+      <c r="N5" s="6">
         <v>0.65</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>79</v>
+      <c r="A6" s="6">
+        <v>6</v>
       </c>
       <c r="B6" s="9">
         <v>11721.3</v>
@@ -75367,27 +75486,37 @@
       <c r="E6" s="9">
         <v>241862797.40000001</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G6" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="J6" s="6">
+        <v>300</v>
+      </c>
+      <c r="K6" s="6">
+        <v>300</v>
+      </c>
+      <c r="L6" s="6">
+        <v>13</v>
+      </c>
+      <c r="M6" s="6">
         <v>7.8090000000000006E-9</v>
       </c>
-      <c r="I6" s="6">
+      <c r="N6" s="6">
         <v>0.65</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>79</v>
+      <c r="A7" s="6">
+        <v>7</v>
       </c>
       <c r="B7" s="9">
         <v>11721.3</v>
@@ -75401,27 +75530,37 @@
       <c r="E7" s="9">
         <v>241862797.40000001</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G7" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H7" s="6">
+      <c r="J7" s="6">
+        <v>300</v>
+      </c>
+      <c r="K7" s="6">
+        <v>300</v>
+      </c>
+      <c r="L7" s="6">
+        <v>13</v>
+      </c>
+      <c r="M7" s="6">
         <v>7.8090000000000006E-9</v>
       </c>
-      <c r="I7" s="6">
+      <c r="N7" s="6">
         <v>0.65</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>79</v>
+      <c r="A8" s="6">
+        <v>8</v>
       </c>
       <c r="B8" s="9">
         <v>11721.3</v>
@@ -75435,27 +75574,37 @@
       <c r="E8" s="9">
         <v>241862797.40000001</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G8" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" s="6">
+      <c r="J8" s="6">
+        <v>300</v>
+      </c>
+      <c r="K8" s="6">
+        <v>300</v>
+      </c>
+      <c r="L8" s="6">
+        <v>13</v>
+      </c>
+      <c r="M8" s="6">
         <v>7.8090000000000006E-9</v>
       </c>
-      <c r="I8" s="6">
+      <c r="N8" s="6">
         <v>0.65</v>
       </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>79</v>
+      <c r="A9" s="6">
+        <v>9</v>
       </c>
       <c r="B9" s="9">
         <v>11721.3</v>
@@ -75469,23 +75618,33 @@
       <c r="E9" s="9">
         <v>241862797.40000001</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G9" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="J9" s="6">
+        <v>300</v>
+      </c>
+      <c r="K9" s="6">
+        <v>300</v>
+      </c>
+      <c r="L9" s="6">
+        <v>13</v>
+      </c>
+      <c r="M9" s="8">
         <v>7.8090000000000006E-9</v>
       </c>
-      <c r="I9" s="6">
+      <c r="N9" s="6">
         <v>0.65</v>
       </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -78231,8 +78390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1761C3A7-822F-4024-B947-737166AA63E5}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se intenta implementar el nuevo marco en la parte de lectura de datos del dr Rolando
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0.xlsx
+++ b/pruebas_excel/marco3Ddam0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD923788-D4FF-4CF8-AF82-876693879AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F50E8A-BCF4-4B20-A153-115825C5B4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1815" windowWidth="24240" windowHeight="13740" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
   </bookViews>
@@ -13597,7 +13597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64754D5-97CF-43AF-A87E-0A6E620C6CCD}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection sqref="A1:D7"/>
@@ -13669,13 +13669,13 @@
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>5000</v>
       </c>
     </row>
@@ -13683,13 +13683,13 @@
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>6000</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>5000</v>
       </c>
     </row>
@@ -14071,6 +14071,16 @@
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correccion de aplicacion de danos locales
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0.xlsx
+++ b/pruebas_excel/marco3Ddam0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F50E8A-BCF4-4B20-A153-115825C5B4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC8BBDC-DF10-40FA-8F27-14E6C7443C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1815" windowWidth="24240" windowHeight="13740" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
+    <workbookView xWindow="29625" yWindow="7320" windowWidth="12000" windowHeight="7995" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="nudos" sheetId="1" r:id="rId1"/>
@@ -78398,15 +78398,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1761C3A7-822F-4024-B947-737166AA63E5}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:H3"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -78428,16 +78428,13 @@
       <c r="G1">
         <v>1</v>
       </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -78454,16 +78451,13 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -78480,11 +78474,8 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integrado la automatizacion de VXZ. Ya se arma la matriz de rigidez. Siguiente paso: comprobar que sea correcta
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0.xlsx
+++ b/pruebas_excel/marco3Ddam0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEDEA9F-5941-4842-8E21-EF502888E374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86410064-5514-47A1-807B-3FDEEFDCAF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29625" yWindow="7320" windowWidth="12000" windowHeight="7995" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
   </bookViews>
@@ -75102,10 +75102,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AD9FD4-C1F6-47BC-8ADE-A0E5BD855E76}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F195"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75116,7 +75116,134 @@
     <col min="5" max="5" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
el marco se cambio uno con 4 elementos, cada uno con el tipo de elemento a analizar, el codigo funciona bien hasta el ensamblaje de matriz de rigidez completa, se comprobaron las deformaciones con unas cargas y si son correctas
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0.xlsx
+++ b/pruebas_excel/marco3Ddam0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86410064-5514-47A1-807B-3FDEEFDCAF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC65C7B-0BFD-43CF-997E-EB4040DB0709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29625" yWindow="7320" windowWidth="12000" windowHeight="7995" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="999" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="nudos" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>Marco 3D</t>
   </si>
@@ -374,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -391,6 +391,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13599,8 +13600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64754D5-97CF-43AF-A87E-0A6E620C6CCD}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:D7"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13628,10 +13629,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -13645,10 +13646,10 @@
         <v>6000</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>5000</v>
+      </c>
+      <c r="D3" s="12">
+        <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -13656,10 +13657,10 @@
         <v>4</v>
       </c>
       <c r="B4">
+        <v>6000</v>
+      </c>
+      <c r="C4">
         <v>0</v>
-      </c>
-      <c r="C4">
-        <v>5000</v>
       </c>
       <c r="D4">
         <v>5000</v>
@@ -13675,37 +13676,14 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>6000</v>
-      </c>
-      <c r="C6">
+      <c r="D5" s="6">
         <v>0</v>
       </c>
-      <c r="D6">
-        <v>5000</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4">
-        <v>6000</v>
-      </c>
-      <c r="C7" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D7" s="4">
-        <v>5000</v>
-      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
@@ -13768,7 +13746,7 @@
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
@@ -74651,22 +74629,22 @@
       </c>
       <c r="N8">
         <f>'prop geom'!B9</f>
-        <v>11721.3</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <v>4000</v>
       </c>
       <c r="P8">
         <f>N8*O8</f>
-        <v>46885200</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="2">
         <f>P8*M8</f>
-        <v>0.11252448</v>
+        <v>0</v>
       </c>
       <c r="R8" s="2">
         <f>Q8/2</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="S8" t="s">
         <v>62</v>
@@ -74774,7 +74752,7 @@
       </c>
       <c r="N12" s="2">
         <f>R8</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -74786,7 +74764,7 @@
       </c>
       <c r="N13" s="2">
         <f>R8+R9+R10</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -74795,7 +74773,7 @@
       </c>
       <c r="N14" s="2">
         <f>R8</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -74804,7 +74782,7 @@
       </c>
       <c r="N15" s="2">
         <f>N13</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -74837,7 +74815,7 @@
       </c>
       <c r="N16" s="2">
         <f>R8</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
@@ -74870,7 +74848,7 @@
       </c>
       <c r="N17" s="2">
         <f>N15</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
@@ -74903,7 +74881,7 @@
       </c>
       <c r="N18" s="2">
         <f>R8</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
@@ -74936,7 +74914,7 @@
       </c>
       <c r="N19" s="2">
         <f>N17</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
@@ -75102,10 +75080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AD9FD4-C1F6-47BC-8ADE-A0E5BD855E76}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection sqref="A1:D9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75122,13 +75100,13 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1">
         <v>0</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -75156,11 +75134,11 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>4</v>
       </c>
       <c r="B4">
@@ -75171,76 +75149,6 @@
       </c>
       <c r="D4">
         <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -75250,10 +75158,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D051BC6-55A0-4B3B-BADC-15C4CA1EE579}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75271,7 +75179,7 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -75282,7 +75190,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -75293,7 +75201,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -75301,65 +75209,10 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
         <v>5</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -75372,7 +75225,7 @@
   <dimension ref="A1:Q182"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:N9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75567,22 +75420,22 @@
       <c r="A5" s="6">
         <v>5</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>11721.3</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>120931398.7</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>120931398.7</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>241862797.40000001</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>199947.98</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>76903.070000000007</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -75608,180 +75461,68 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>6</v>
-      </c>
-      <c r="B6" s="9">
-        <v>11721.3</v>
-      </c>
-      <c r="C6" s="9">
-        <v>120931398.7</v>
-      </c>
-      <c r="D6" s="9">
-        <v>120931398.7</v>
-      </c>
-      <c r="E6" s="9">
-        <v>241862797.40000001</v>
-      </c>
-      <c r="F6" s="9">
-        <v>199947.98</v>
-      </c>
-      <c r="G6" s="9">
-        <v>76903.070000000007</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="J6" s="6">
-        <v>300</v>
-      </c>
-      <c r="K6" s="6">
-        <v>300</v>
-      </c>
-      <c r="L6" s="6">
-        <v>13</v>
-      </c>
-      <c r="M6" s="6">
-        <v>7.8090000000000006E-9</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0.65</v>
-      </c>
+      <c r="A6" s="6"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>7</v>
-      </c>
-      <c r="B7" s="9">
-        <v>11721.3</v>
-      </c>
-      <c r="C7" s="9">
-        <v>120931398.7</v>
-      </c>
-      <c r="D7" s="9">
-        <v>120931398.7</v>
-      </c>
-      <c r="E7" s="9">
-        <v>241862797.40000001</v>
-      </c>
-      <c r="F7" s="9">
-        <v>199947.98</v>
-      </c>
-      <c r="G7" s="9">
-        <v>76903.070000000007</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="6">
-        <v>300</v>
-      </c>
-      <c r="K7" s="6">
-        <v>300</v>
-      </c>
-      <c r="L7" s="6">
-        <v>13</v>
-      </c>
-      <c r="M7" s="6">
-        <v>7.8090000000000006E-9</v>
-      </c>
-      <c r="N7" s="6">
-        <v>0.65</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>8</v>
-      </c>
-      <c r="B8" s="9">
-        <v>11721.3</v>
-      </c>
-      <c r="C8" s="9">
-        <v>120931398.7</v>
-      </c>
-      <c r="D8" s="9">
-        <v>120931398.7</v>
-      </c>
-      <c r="E8" s="9">
-        <v>241862797.40000001</v>
-      </c>
-      <c r="F8" s="9">
-        <v>199947.98</v>
-      </c>
-      <c r="G8" s="9">
-        <v>76903.070000000007</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" s="6">
-        <v>300</v>
-      </c>
-      <c r="K8" s="6">
-        <v>300</v>
-      </c>
-      <c r="L8" s="6">
-        <v>13</v>
-      </c>
-      <c r="M8" s="6">
-        <v>7.8090000000000006E-9</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0.65</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>9</v>
-      </c>
-      <c r="B9" s="9">
-        <v>11721.3</v>
-      </c>
-      <c r="C9" s="9">
-        <v>120931398.7</v>
-      </c>
-      <c r="D9" s="9">
-        <v>120931398.7</v>
-      </c>
-      <c r="E9" s="9">
-        <v>241862797.40000001</v>
-      </c>
-      <c r="F9" s="9">
-        <v>199947.98</v>
-      </c>
-      <c r="G9" s="9">
-        <v>76903.070000000007</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="J9" s="6">
-        <v>300</v>
-      </c>
-      <c r="K9" s="6">
-        <v>300</v>
-      </c>
-      <c r="L9" s="6">
-        <v>13</v>
-      </c>
-      <c r="M9" s="8">
-        <v>7.8090000000000006E-9</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0.65</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -78514,7 +78255,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78527,8 +78268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1761C3A7-822F-4024-B947-737166AA63E5}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:G3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78553,52 +78294,6 @@
         <v>1</v>
       </c>
       <c r="G1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
         <v>1</v>
       </c>
     </row>
@@ -78680,7 +78375,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
correccion del numero de daños al inicio del codigo
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0.xlsx
+++ b/pruebas_excel/marco3Ddam0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEDEA9F-5941-4842-8E21-EF502888E374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB09DA5B-0CCB-4B2F-B744-59A1F5DF5E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29625" yWindow="7320" windowWidth="12000" windowHeight="7995" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="nudos" sheetId="1" r:id="rId1"/>
@@ -13600,7 +13600,7 @@
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:D7"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13620,7 +13620,7 @@
         <v>5000</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -13628,10 +13628,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -13645,10 +13645,10 @@
         <v>6000</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -13656,13 +13656,13 @@
         <v>4</v>
       </c>
       <c r="B4">
+        <v>6000</v>
+      </c>
+      <c r="C4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>5000</v>
-      </c>
       <c r="D4">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -13673,10 +13673,10 @@
         <v>0</v>
       </c>
       <c r="C5">
+        <v>5000</v>
+      </c>
+      <c r="D5">
         <v>0</v>
-      </c>
-      <c r="D5">
-        <v>5000</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -13684,13 +13684,13 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -13698,19 +13698,28 @@
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="C7" s="4">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D7" s="4">
         <v>5000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>6000</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5000</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
@@ -75102,10 +75111,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AD9FD4-C1F6-47BC-8ADE-A0E5BD855E76}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:F195"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75116,7 +75125,134 @@
     <col min="5" max="5" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -75144,7 +75280,7 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -75155,7 +75291,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -75163,10 +75299,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -75174,7 +75310,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -75185,10 +75321,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -75196,10 +75332,10 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -75207,10 +75343,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -75218,10 +75354,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -75229,10 +75365,10 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -78401,14 +78537,14 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -78454,7 +78590,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -78472,6 +78608,29 @@
         <v>1</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
marco simetrico de 1 nivel con diagonales simetricas donde las diagonales son los unicos identificados
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0.xlsx
+++ b/pruebas_excel/marco3Ddam0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BE86D2-7A2A-4C9A-8F64-C7D3533E4446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E9CFB6-C992-4499-BAEF-B0840A489DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
+    <workbookView xWindow="31800" yWindow="4530" windowWidth="12000" windowHeight="7995" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="nudos" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="81">
   <si>
     <t>Marco 3D</t>
   </si>
@@ -13600,7 +13600,7 @@
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:D8"/>
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13614,13 +13614,13 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="C1">
         <v>5000</v>
       </c>
       <c r="D1">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -13628,7 +13628,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>5000</v>
@@ -13642,13 +13642,13 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -13670,13 +13670,13 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="C5">
         <v>5000</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -13687,10 +13687,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -13698,13 +13698,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
       </c>
       <c r="D7" s="4">
-        <v>5000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -13715,31 +13715,67 @@
         <v>6000</v>
       </c>
       <c r="C8" s="4">
+        <v>2500</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>6000</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
         <v>0</v>
       </c>
-      <c r="D8" s="4">
+      <c r="C10" s="4">
         <v>5000</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4">
+        <v>5000</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5000</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4">
+        <v>6000</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5000</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
@@ -74724,22 +74760,22 @@
       </c>
       <c r="N9">
         <f>'prop geom'!B11</f>
-        <v>0</v>
+        <v>11721.3</v>
       </c>
       <c r="O9">
         <v>6000</v>
       </c>
       <c r="P9">
         <f>N9*O9</f>
-        <v>0</v>
+        <v>70327800</v>
       </c>
       <c r="Q9" s="2">
         <f>P9*M9</f>
-        <v>0</v>
+        <v>0.16878672</v>
       </c>
       <c r="R9" s="2">
         <f>Q9/2</f>
-        <v>0</v>
+        <v>8.4393360000000001E-2</v>
       </c>
       <c r="S9" t="s">
         <v>64</v>
@@ -74751,22 +74787,22 @@
       </c>
       <c r="N10">
         <f>'prop geom'!B14</f>
-        <v>0</v>
+        <v>11721.3</v>
       </c>
       <c r="O10">
         <v>5000</v>
       </c>
       <c r="P10">
         <f>N10*O10</f>
-        <v>0</v>
+        <v>58606500</v>
       </c>
       <c r="Q10" s="2">
         <f>P10*M10</f>
-        <v>0</v>
+        <v>0.14065559999999999</v>
       </c>
       <c r="R10" s="2">
         <f>Q10/2</f>
-        <v>0</v>
+        <v>7.0327799999999996E-2</v>
       </c>
       <c r="S10" t="s">
         <v>65</v>
@@ -74795,7 +74831,7 @@
       </c>
       <c r="N13" s="2">
         <f>R8+R9+R10</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0.21098339999999999</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -74813,7 +74849,7 @@
       </c>
       <c r="N15" s="2">
         <f>N13</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0.21098339999999999</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -74879,7 +74915,7 @@
       </c>
       <c r="N17" s="2">
         <f>N15</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0.21098339999999999</v>
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
@@ -74945,7 +74981,7 @@
       </c>
       <c r="N19" s="2">
         <f>N17</f>
-        <v>5.6262239999999998E-2</v>
+        <v>0.21098339999999999</v>
       </c>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
@@ -75111,10 +75147,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AD9FD4-C1F6-47BC-8ADE-A0E5BD855E76}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:D9"/>
+      <selection sqref="A1:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75137,7 +75173,7 @@
         <v>0</v>
       </c>
       <c r="D1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -75145,7 +75181,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -75159,7 +75195,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -75173,7 +75209,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -75207,7 +75243,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -75221,7 +75257,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -75235,7 +75271,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -75250,6 +75286,216 @@
       </c>
       <c r="D9">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -75259,10 +75505,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D051BC6-55A0-4B3B-BADC-15C4CA1EE579}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75277,10 +75523,10 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -75288,10 +75534,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -75299,10 +75545,10 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -75310,10 +75556,10 @@
         <v>4</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>6</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -75321,10 +75567,10 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -75332,10 +75578,10 @@
         <v>6</v>
       </c>
       <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>7</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -75346,7 +75592,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -75354,10 +75600,10 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -75365,10 +75611,175 @@
         <v>9</v>
       </c>
       <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
         <v>2</v>
       </c>
-      <c r="C9">
-        <v>1</v>
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -75381,7 +75792,7 @@
   <dimension ref="A1:Q182"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:N9"/>
+      <selection sqref="A1:N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75793,244 +76204,664 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="6"/>
+      <c r="A10" s="6">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C10" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D10" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E10" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F10" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G10" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="6">
+        <v>300</v>
+      </c>
+      <c r="K10" s="6">
+        <v>300</v>
+      </c>
+      <c r="L10" s="6">
+        <v>13</v>
+      </c>
+      <c r="M10" s="8">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N10" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="6"/>
+      <c r="A11" s="6">
+        <v>11</v>
+      </c>
+      <c r="B11" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C11" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D11" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E11" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F11" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G11" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="6">
+        <v>300</v>
+      </c>
+      <c r="K11" s="6">
+        <v>300</v>
+      </c>
+      <c r="L11" s="6">
+        <v>13</v>
+      </c>
+      <c r="M11" s="8">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="6"/>
+      <c r="A12" s="6">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C12" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D12" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E12" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F12" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G12" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" s="6">
+        <v>300</v>
+      </c>
+      <c r="K12" s="6">
+        <v>300</v>
+      </c>
+      <c r="L12" s="6">
+        <v>13</v>
+      </c>
+      <c r="M12" s="8">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N12" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="6"/>
+      <c r="A13" s="6">
+        <v>13</v>
+      </c>
+      <c r="B13" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C13" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D13" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E13" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F13" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G13" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="6">
+        <v>300</v>
+      </c>
+      <c r="K13" s="6">
+        <v>300</v>
+      </c>
+      <c r="L13" s="6">
+        <v>13</v>
+      </c>
+      <c r="M13" s="8">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="6"/>
+      <c r="A14" s="6">
+        <v>14</v>
+      </c>
+      <c r="B14" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C14" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D14" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E14" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F14" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G14" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="6">
+        <v>300</v>
+      </c>
+      <c r="K14" s="6">
+        <v>300</v>
+      </c>
+      <c r="L14" s="6">
+        <v>13</v>
+      </c>
+      <c r="M14" s="8">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N14" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="6"/>
+      <c r="A15" s="10">
+        <v>15</v>
+      </c>
+      <c r="B15" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C15" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D15" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E15" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F15" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G15" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="6">
+        <v>300</v>
+      </c>
+      <c r="K15" s="6">
+        <v>300</v>
+      </c>
+      <c r="L15" s="6">
+        <v>13</v>
+      </c>
+      <c r="M15" s="8">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N15" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="6"/>
+      <c r="A16" s="10">
+        <v>16</v>
+      </c>
+      <c r="B16" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C16" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D16" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E16" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F16" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G16" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J16" s="6">
+        <v>300</v>
+      </c>
+      <c r="K16" s="6">
+        <v>300</v>
+      </c>
+      <c r="L16" s="6">
+        <v>13</v>
+      </c>
+      <c r="M16" s="8">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N16" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
+      <c r="A17" s="10">
+        <v>17</v>
+      </c>
+      <c r="B17" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C17" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D17" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E17" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F17" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G17" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="6">
+        <v>300</v>
+      </c>
+      <c r="K17" s="6">
+        <v>300</v>
+      </c>
+      <c r="L17" s="6">
+        <v>13</v>
+      </c>
+      <c r="M17" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N17" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
+      <c r="A18" s="10">
+        <v>18</v>
+      </c>
+      <c r="B18" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C18" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D18" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E18" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F18" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G18" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="6">
+        <v>300</v>
+      </c>
+      <c r="K18" s="6">
+        <v>300</v>
+      </c>
+      <c r="L18" s="6">
+        <v>13</v>
+      </c>
+      <c r="M18" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N18" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
+      <c r="A19" s="10">
+        <v>19</v>
+      </c>
+      <c r="B19" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C19" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D19" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E19" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F19" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G19" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="6">
+        <v>300</v>
+      </c>
+      <c r="K19" s="6">
+        <v>300</v>
+      </c>
+      <c r="L19" s="6">
+        <v>13</v>
+      </c>
+      <c r="M19" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
+      <c r="A20" s="10">
+        <v>20</v>
+      </c>
+      <c r="B20" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C20" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D20" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E20" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F20" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G20" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="6">
+        <v>300</v>
+      </c>
+      <c r="K20" s="6">
+        <v>300</v>
+      </c>
+      <c r="L20" s="6">
+        <v>13</v>
+      </c>
+      <c r="M20" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N20" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
+      <c r="A21" s="10">
+        <v>21</v>
+      </c>
+      <c r="B21" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C21" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D21" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E21" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F21" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G21" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="6">
+        <v>300</v>
+      </c>
+      <c r="K21" s="6">
+        <v>300</v>
+      </c>
+      <c r="L21" s="6">
+        <v>13</v>
+      </c>
+      <c r="M21" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
+      <c r="A22" s="10">
+        <v>22</v>
+      </c>
+      <c r="B22" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C22" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D22" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E22" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F22" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G22" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" s="6">
+        <v>300</v>
+      </c>
+      <c r="K22" s="6">
+        <v>300</v>
+      </c>
+      <c r="L22" s="6">
+        <v>13</v>
+      </c>
+      <c r="M22" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
+      <c r="A23" s="6">
+        <v>23</v>
+      </c>
+      <c r="B23" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C23" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D23" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E23" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F23" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G23" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J23" s="6">
+        <v>300</v>
+      </c>
+      <c r="K23" s="6">
+        <v>300</v>
+      </c>
+      <c r="L23" s="6">
+        <v>13</v>
+      </c>
+      <c r="M23" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N23" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
+      <c r="A24" s="6">
+        <v>24</v>
+      </c>
+      <c r="B24" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C24" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D24" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E24" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F24" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G24" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J24" s="6">
+        <v>300</v>
+      </c>
+      <c r="K24" s="6">
+        <v>300</v>
+      </c>
+      <c r="L24" s="6">
+        <v>13</v>
+      </c>
+      <c r="M24" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N24" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
@@ -78544,7 +79375,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -78567,7 +79398,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -78613,7 +79444,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>1</v>

</xml_diff>

<commit_message>
el AG identifica daños en columnas y en diagonales, ya se me integro el MAC con pesos 50 y 50. 50 para las frecuencias y 50 para las formas mediante el MAC
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0.xlsx
+++ b/pruebas_excel/marco3Ddam0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Archivos_Jaret\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E9CFB6-C992-4499-BAEF-B0840A489DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2617A74-93B7-4937-8D4D-6C10ACBF1633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31800" yWindow="4530" windowWidth="12000" windowHeight="7995" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="999" activeTab="5" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="nudos" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="81">
   <si>
     <t>Marco 3D</t>
   </si>
@@ -13600,7 +13600,7 @@
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:D12"/>
+      <selection sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13778,101 +13778,173 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>7500</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>6000</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2500</v>
+      </c>
+      <c r="D14" s="4">
+        <v>7500</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D15" s="4">
+        <v>7500</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2500</v>
+      </c>
+      <c r="D16" s="4">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D17" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4">
+        <v>6000</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4">
+        <v>6000</v>
+      </c>
+      <c r="C20" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D20" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -75147,10 +75219,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AD9FD4-C1F6-47BC-8ADE-A0E5BD855E76}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:D24"/>
+      <selection sqref="A1:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75498,6 +75570,342 @@
         <v>1</v>
       </c>
     </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75505,10 +75913,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D051BC6-55A0-4B3B-BADC-15C4CA1EE579}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:C24"/>
+      <selection sqref="A1:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75782,6 +76190,270 @@
         <v>9</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>13</v>
+      </c>
+      <c r="C27">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>16</v>
+      </c>
+      <c r="C41">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>16</v>
+      </c>
+      <c r="C43">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>18</v>
+      </c>
+      <c r="C45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>19</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>17</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75792,7 +76464,7 @@
   <dimension ref="A1:Q182"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:N24"/>
+      <selection sqref="A1:N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -76864,388 +77536,1060 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
+      <c r="A25" s="6">
+        <v>25</v>
+      </c>
+      <c r="B25" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C25" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D25" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E25" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F25" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G25" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" s="6">
+        <v>300</v>
+      </c>
+      <c r="K25" s="6">
+        <v>300</v>
+      </c>
+      <c r="L25" s="6">
+        <v>13</v>
+      </c>
+      <c r="M25" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N25" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
+      <c r="A26" s="6">
+        <v>26</v>
+      </c>
+      <c r="B26" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C26" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D26" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E26" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F26" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G26" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26" s="6">
+        <v>300</v>
+      </c>
+      <c r="K26" s="6">
+        <v>300</v>
+      </c>
+      <c r="L26" s="6">
+        <v>13</v>
+      </c>
+      <c r="M26" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N26" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
+      <c r="A27" s="6">
+        <v>27</v>
+      </c>
+      <c r="B27" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C27" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D27" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E27" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F27" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G27" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J27" s="6">
+        <v>300</v>
+      </c>
+      <c r="K27" s="6">
+        <v>300</v>
+      </c>
+      <c r="L27" s="6">
+        <v>13</v>
+      </c>
+      <c r="M27" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N27" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
+      <c r="A28" s="6">
+        <v>28</v>
+      </c>
+      <c r="B28" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C28" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D28" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E28" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F28" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G28" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J28" s="6">
+        <v>300</v>
+      </c>
+      <c r="K28" s="6">
+        <v>300</v>
+      </c>
+      <c r="L28" s="6">
+        <v>13</v>
+      </c>
+      <c r="M28" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N28" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
+      <c r="A29" s="6">
+        <v>29</v>
+      </c>
+      <c r="B29" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C29" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D29" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E29" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F29" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G29" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J29" s="6">
+        <v>300</v>
+      </c>
+      <c r="K29" s="6">
+        <v>300</v>
+      </c>
+      <c r="L29" s="6">
+        <v>13</v>
+      </c>
+      <c r="M29" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N29" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
+      <c r="A30" s="6">
+        <v>30</v>
+      </c>
+      <c r="B30" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C30" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D30" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E30" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F30" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G30" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30" s="6">
+        <v>300</v>
+      </c>
+      <c r="K30" s="6">
+        <v>300</v>
+      </c>
+      <c r="L30" s="6">
+        <v>13</v>
+      </c>
+      <c r="M30" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N30" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
+      <c r="A31" s="6">
+        <v>31</v>
+      </c>
+      <c r="B31" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C31" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D31" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E31" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F31" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G31" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J31" s="6">
+        <v>300</v>
+      </c>
+      <c r="K31" s="6">
+        <v>300</v>
+      </c>
+      <c r="L31" s="6">
+        <v>13</v>
+      </c>
+      <c r="M31" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N31" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
+      <c r="A32" s="6">
+        <v>32</v>
+      </c>
+      <c r="B32" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C32" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D32" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E32" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F32" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G32" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J32" s="6">
+        <v>300</v>
+      </c>
+      <c r="K32" s="6">
+        <v>300</v>
+      </c>
+      <c r="L32" s="6">
+        <v>13</v>
+      </c>
+      <c r="M32" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N32" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
+      <c r="A33" s="6">
+        <v>33</v>
+      </c>
+      <c r="B33" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C33" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D33" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E33" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F33" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G33" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J33" s="6">
+        <v>300</v>
+      </c>
+      <c r="K33" s="6">
+        <v>300</v>
+      </c>
+      <c r="L33" s="6">
+        <v>13</v>
+      </c>
+      <c r="M33" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N33" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
+      <c r="A34" s="6">
+        <v>34</v>
+      </c>
+      <c r="B34" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C34" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D34" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E34" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F34" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G34" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J34" s="6">
+        <v>300</v>
+      </c>
+      <c r="K34" s="6">
+        <v>300</v>
+      </c>
+      <c r="L34" s="6">
+        <v>13</v>
+      </c>
+      <c r="M34" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N34" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
+      <c r="A35" s="6">
+        <v>35</v>
+      </c>
+      <c r="B35" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C35" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D35" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E35" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F35" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G35" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J35" s="6">
+        <v>300</v>
+      </c>
+      <c r="K35" s="6">
+        <v>300</v>
+      </c>
+      <c r="L35" s="6">
+        <v>13</v>
+      </c>
+      <c r="M35" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N35" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
+      <c r="A36" s="6">
+        <v>36</v>
+      </c>
+      <c r="B36" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C36" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D36" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E36" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F36" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G36" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J36" s="6">
+        <v>300</v>
+      </c>
+      <c r="K36" s="6">
+        <v>300</v>
+      </c>
+      <c r="L36" s="6">
+        <v>13</v>
+      </c>
+      <c r="M36" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N36" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
+      <c r="A37" s="6">
+        <v>37</v>
+      </c>
+      <c r="B37" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C37" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D37" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E37" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F37" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G37" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J37" s="6">
+        <v>300</v>
+      </c>
+      <c r="K37" s="6">
+        <v>300</v>
+      </c>
+      <c r="L37" s="6">
+        <v>13</v>
+      </c>
+      <c r="M37" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N37" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
+      <c r="A38" s="6">
+        <v>38</v>
+      </c>
+      <c r="B38" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C38" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D38" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E38" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F38" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G38" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J38" s="6">
+        <v>300</v>
+      </c>
+      <c r="K38" s="6">
+        <v>300</v>
+      </c>
+      <c r="L38" s="6">
+        <v>13</v>
+      </c>
+      <c r="M38" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N38" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
+      <c r="A39" s="6">
+        <v>39</v>
+      </c>
+      <c r="B39" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C39" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D39" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E39" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F39" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G39" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J39" s="6">
+        <v>300</v>
+      </c>
+      <c r="K39" s="6">
+        <v>300</v>
+      </c>
+      <c r="L39" s="6">
+        <v>13</v>
+      </c>
+      <c r="M39" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N39" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
+      <c r="A40" s="6">
+        <v>40</v>
+      </c>
+      <c r="B40" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C40" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D40" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E40" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F40" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G40" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J40" s="6">
+        <v>300</v>
+      </c>
+      <c r="K40" s="6">
+        <v>300</v>
+      </c>
+      <c r="L40" s="6">
+        <v>13</v>
+      </c>
+      <c r="M40" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N40" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
+      <c r="A41" s="6">
+        <v>41</v>
+      </c>
+      <c r="B41" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C41" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D41" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E41" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F41" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G41" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J41" s="6">
+        <v>300</v>
+      </c>
+      <c r="K41" s="6">
+        <v>300</v>
+      </c>
+      <c r="L41" s="6">
+        <v>13</v>
+      </c>
+      <c r="M41" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N41" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
+      <c r="A42" s="6">
+        <v>42</v>
+      </c>
+      <c r="B42" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C42" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D42" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E42" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F42" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G42" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J42" s="6">
+        <v>300</v>
+      </c>
+      <c r="K42" s="6">
+        <v>300</v>
+      </c>
+      <c r="L42" s="6">
+        <v>13</v>
+      </c>
+      <c r="M42" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N42" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
+      <c r="A43" s="6">
+        <v>43</v>
+      </c>
+      <c r="B43" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C43" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D43" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E43" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F43" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G43" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J43" s="6">
+        <v>300</v>
+      </c>
+      <c r="K43" s="6">
+        <v>300</v>
+      </c>
+      <c r="L43" s="6">
+        <v>13</v>
+      </c>
+      <c r="M43" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N43" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
+      <c r="A44" s="6">
+        <v>44</v>
+      </c>
+      <c r="B44" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C44" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D44" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E44" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F44" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G44" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J44" s="6">
+        <v>300</v>
+      </c>
+      <c r="K44" s="6">
+        <v>300</v>
+      </c>
+      <c r="L44" s="6">
+        <v>13</v>
+      </c>
+      <c r="M44" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N44" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
+      <c r="A45" s="6">
+        <v>45</v>
+      </c>
+      <c r="B45" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C45" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D45" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E45" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F45" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G45" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J45" s="6">
+        <v>300</v>
+      </c>
+      <c r="K45" s="6">
+        <v>300</v>
+      </c>
+      <c r="L45" s="6">
+        <v>13</v>
+      </c>
+      <c r="M45" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N45" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6"/>
+      <c r="A46" s="6">
+        <v>46</v>
+      </c>
+      <c r="B46" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C46" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D46" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E46" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F46" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G46" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J46" s="6">
+        <v>300</v>
+      </c>
+      <c r="K46" s="6">
+        <v>300</v>
+      </c>
+      <c r="L46" s="6">
+        <v>13</v>
+      </c>
+      <c r="M46" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N46" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
+      <c r="A47" s="6">
+        <v>47</v>
+      </c>
+      <c r="B47" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C47" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D47" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E47" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F47" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G47" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J47" s="6">
+        <v>300</v>
+      </c>
+      <c r="K47" s="6">
+        <v>300</v>
+      </c>
+      <c r="L47" s="6">
+        <v>13</v>
+      </c>
+      <c r="M47" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N47" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
+      <c r="A48" s="6">
+        <v>48</v>
+      </c>
+      <c r="B48" s="9">
+        <v>11721.3</v>
+      </c>
+      <c r="C48" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="D48" s="9">
+        <v>120931398.7</v>
+      </c>
+      <c r="E48" s="9">
+        <v>241862797.40000001</v>
+      </c>
+      <c r="F48" s="9">
+        <v>199947.98</v>
+      </c>
+      <c r="G48" s="9">
+        <v>76903.070000000007</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J48" s="6">
+        <v>300</v>
+      </c>
+      <c r="K48" s="6">
+        <v>300</v>
+      </c>
+      <c r="L48" s="6">
+        <v>13</v>
+      </c>
+      <c r="M48" s="6">
+        <v>7.8090000000000006E-9</v>
+      </c>
+      <c r="N48" s="6">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>

</xml_diff>

<commit_message>
integracion de la longitud del arco
</commit_message>
<xml_diff>
--- a/pruebas_excel/marco3Ddam0.xlsx
+++ b/pruebas_excel/marco3Ddam0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2e5581da9410f33/Documentos/MATLAB/Proyecto-doctoral/pruebas_excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP.DESKTOP-LLLQP6U\Documents\Proyecto-doctoral\pruebas_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{50FD523D-E5D4-4960-A3E5-51651AE75168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B141E69-5FEC-4862-B239-0F46E6236485}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295C6F46-4849-4BA5-A732-6DF21119A4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" tabRatio="999" activeTab="1" xr2:uid="{DB4B52A0-7431-4402-AD95-01FEF59D5D3F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="999" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nudos" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="damage" sheetId="14" r:id="rId13"/>
     <sheet name="opensees" sheetId="8" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,6 +40,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -13597,144 +13599,393 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64754D5-97CF-43AF-A87E-0A6E620C6CCD}">
-  <dimension ref="B7:D82"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection sqref="A1:MB500"/>
+      <selection sqref="A1:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="4" width="9"/>
     <col min="5" max="5" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9"/>
     <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>41666.67</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>41666.67</v>
+      </c>
+      <c r="C3">
+        <v>41666.660000000003</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>41666.660000000003</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>20833.330000000002</v>
+      </c>
+      <c r="C5">
+        <v>1329.79</v>
+      </c>
+      <c r="D5">
+        <v>10638.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>40336.879999999997</v>
+      </c>
+      <c r="C6">
+        <v>20833.330000000002</v>
+      </c>
+      <c r="D6">
+        <v>10638.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>20833.330000000002</v>
+      </c>
+      <c r="C7" s="4">
+        <v>40336.870000000003</v>
+      </c>
+      <c r="D7" s="4">
+        <v>10638.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1329.79</v>
+      </c>
+      <c r="C8" s="4">
+        <v>20833.330000000002</v>
+      </c>
+      <c r="D8" s="4">
+        <v>10638.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2500</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2500</v>
+      </c>
+      <c r="D9" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
+        <v>39166.67</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2500</v>
+      </c>
+      <c r="D10" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4">
+        <v>39166.67</v>
+      </c>
+      <c r="C11" s="4">
+        <v>39166.660000000003</v>
+      </c>
+      <c r="D11" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4">
+        <v>2500</v>
+      </c>
+      <c r="C12" s="4">
+        <v>39166.660000000003</v>
+      </c>
+      <c r="D12" s="4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4">
+        <v>20833.330000000002</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3841.46</v>
+      </c>
+      <c r="D13" s="4">
+        <v>30731.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>37825.199999999997</v>
+      </c>
+      <c r="C14" s="4">
+        <v>20833.330000000002</v>
+      </c>
+      <c r="D14" s="4">
+        <v>30731.71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4">
+        <v>20833.330000000002</v>
+      </c>
+      <c r="C15" s="4">
+        <v>37825.199999999997</v>
+      </c>
+      <c r="D15" s="4">
+        <v>30731.71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>3841.46</v>
+      </c>
+      <c r="C16" s="4">
+        <v>20833.330000000002</v>
+      </c>
+      <c r="D16" s="4">
+        <v>30731.71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D17" s="4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
+        <v>36666.67</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D18" s="4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4">
+        <v>36666.67</v>
+      </c>
+      <c r="C19" s="4">
+        <v>36666.660000000003</v>
+      </c>
+      <c r="D19" s="4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C20" s="4">
+        <v>36666.660000000003</v>
+      </c>
+      <c r="D20" s="4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C21" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D21" s="4">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4">
+        <v>36666.67</v>
+      </c>
+      <c r="C22" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D22" s="4">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" s="4">
+        <v>36666.67</v>
+      </c>
+      <c r="C23" s="4">
+        <v>36666.660000000003</v>
+      </c>
+      <c r="D23" s="4">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C24" s="4">
+        <v>36666.660000000003</v>
+      </c>
+      <c r="D24" s="4">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -14005,6 +14256,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9"/>
     <col min="2" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="0.88671875" customWidth="1"/>
@@ -75009,10 +75261,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AD9FD4-C1F6-47BC-8ADE-A0E5BD855E76}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:MB500"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -75022,8 +75274,794 @@
     <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -75041,6 +76079,7 @@
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -75680,7 +76719,9 @@
     <col min="4" max="4" width="21.5546875" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9"/>
     <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="14" width="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.6">
@@ -80140,11 +81181,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1761C3A7-822F-4024-B947-737166AA63E5}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="10" width="9"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">

</xml_diff>